<commit_message>
First Release with both Phases 1 and 2
</commit_message>
<xml_diff>
--- a/c_module/FingerprintClassification/Charts/Phase1.xlsx
+++ b/c_module/FingerprintClassification/Charts/Phase1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="17">
   <si>
     <t>201503.csv</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Prediction</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>NBIS3.0.0</t>
+  </si>
+  <si>
+    <t>NBIS.NET(5)</t>
   </si>
 </sst>
 </file>
@@ -89,7 +98,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -208,11 +217,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -232,6 +272,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,16 +555,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:I42"/>
+  <dimension ref="A3:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="Q33" sqref="Q33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -539,8 +583,12 @@
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5" t="s">
@@ -719,8 +767,12 @@
       <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="13" t="s">
@@ -752,7 +804,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="6"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -771,7 +823,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="6"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -786,7 +838,7 @@
       </c>
       <c r="I18" s="6"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -809,7 +861,7 @@
         <v>0.605020920502092</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -832,7 +884,7 @@
         <v>0.22719665271966527</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -855,7 +907,7 @@
         <v>2.0502092050209204E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -878,7 +930,7 @@
         <v>0.14728033472803348</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -889,7 +941,7 @@
       <c r="H23" s="16"/>
       <c r="I23" s="18"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -899,10 +951,23 @@
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="6"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20"/>
+      <c r="O24" s="20"/>
+      <c r="P24" s="20"/>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="21"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
@@ -914,8 +979,25 @@
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
       <c r="I25" s="6"/>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="5">
+        <v>3209</v>
+      </c>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="6"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -933,8 +1015,25 @@
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="6"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="4"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="O26" s="5">
+        <f>O29+O32</f>
+        <v>2499</v>
+      </c>
+      <c r="P26" s="7">
+        <f>O26/$F$25</f>
+        <v>0.77874727329386106</v>
+      </c>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="6"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
@@ -952,8 +1051,25 @@
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="4"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O27" s="5">
+        <f>O30+O31</f>
+        <v>710</v>
+      </c>
+      <c r="P27" s="7">
+        <f>O27/$F$25</f>
+        <v>0.22125272670613899</v>
+      </c>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="6"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
@@ -967,8 +1083,21 @@
         <v>6</v>
       </c>
       <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="4"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="R28" s="6"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -990,8 +1119,29 @@
         <f>H29/$F$25</f>
         <v>0.64724213150514176</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="4"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="O29" s="5">
+        <v>1760</v>
+      </c>
+      <c r="P29" s="7">
+        <f>O29/$F$25</f>
+        <v>0.54845746338423185</v>
+      </c>
+      <c r="Q29" s="5">
+        <v>2026</v>
+      </c>
+      <c r="R29" s="12">
+        <f>Q29/$F$25</f>
+        <v>0.63134933000934867</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1013,8 +1163,29 @@
         <f>H30/$F$25</f>
         <v>0.19569959488937363</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="4"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" s="5">
+        <v>612</v>
+      </c>
+      <c r="P30" s="7">
+        <f>O30/$F$25</f>
+        <v>0.19071361794951699</v>
+      </c>
+      <c r="Q30" s="5">
+        <v>639</v>
+      </c>
+      <c r="R30" s="12">
+        <f>Q30/$F$25</f>
+        <v>0.19912745403552509</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1036,8 +1207,29 @@
         <f>H31/$F$25</f>
         <v>2.5553131816765346E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="4"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O31" s="5">
+        <v>98</v>
+      </c>
+      <c r="P31" s="7">
+        <f>O31/$F$25</f>
+        <v>3.0539108756622E-2</v>
+      </c>
+      <c r="Q31" s="5">
+        <v>71</v>
+      </c>
+      <c r="R31" s="12">
+        <f>Q31/$F$25</f>
+        <v>2.2125272670613899E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
@@ -1058,6 +1250,27 @@
       <c r="I32" s="14">
         <f>H32/$F$25</f>
         <v>0.13150514178871922</v>
+      </c>
+      <c r="J32" s="8"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O32" s="9">
+        <v>739</v>
+      </c>
+      <c r="P32" s="10">
+        <f>O32/$F$25</f>
+        <v>0.23028980990962916</v>
+      </c>
+      <c r="Q32" s="9">
+        <v>473</v>
+      </c>
+      <c r="R32" s="14">
+        <f>Q32/$F$25</f>
+        <v>0.14739794328451231</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1109,8 +1322,12 @@
       <c r="I36" s="6"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">

</xml_diff>